<commit_message>
altera nomenclatura da planilha xls
</commit_message>
<xml_diff>
--- a/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
+++ b/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\.CGE\transparencia-mg\acordo-judicial-reparacao-vale-projetos\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D332FA3B-0DA0-420C-B859-E3FE121F8D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A377FA-5AB7-4CE8-A058-B288DDD9B75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="867" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,9 +46,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
   <si>
-    <t>projeto</t>
-  </si>
-  <si>
     <t>anexo</t>
   </si>
   <si>
@@ -257,6 +254,9 @@
   </si>
   <si>
     <t>valor_iniciativa</t>
+  </si>
+  <si>
+    <t>iniciativa</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,16 +654,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -671,10 +671,10 @@
         <v>9288130</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="5">
         <v>1195796000</v>
@@ -685,10 +685,10 @@
         <v>9288130</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
       <c r="D3" s="5">
         <v>450000000</v>
@@ -699,10 +699,10 @@
         <v>9288132</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5">
         <v>270000000</v>
@@ -713,10 +713,10 @@
         <v>9288133</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5">
         <v>776000000</v>
@@ -727,10 +727,10 @@
         <v>9288134</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5">
         <v>118860000</v>
@@ -741,10 +741,10 @@
         <v>9288135</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="5">
         <v>1345000</v>
@@ -755,10 +755,10 @@
         <v>9288136</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5">
         <v>111480000</v>
@@ -769,10 +769,10 @@
         <v>9288137</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="5">
         <v>98100000</v>
@@ -783,10 +783,10 @@
         <v>9288138</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="5">
         <v>38614000</v>
@@ -797,10 +797,10 @@
         <v>9288139</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="5">
         <v>4400000</v>
@@ -811,10 +811,10 @@
         <v>9288141</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="5">
         <v>500000</v>
@@ -825,10 +825,10 @@
         <v>9288142</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="5">
         <v>36712000</v>
@@ -839,10 +839,10 @@
         <v>9288143</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="5">
         <v>728000</v>
@@ -853,10 +853,10 @@
         <v>9288144</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="5">
         <v>49000000</v>
@@ -867,10 +867,10 @@
         <v>9288145</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="5">
         <v>45345000</v>
@@ -881,10 +881,10 @@
         <v>9288147</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" s="5">
         <v>14817323</v>
@@ -895,10 +895,10 @@
         <v>9288148</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="5">
         <v>4000000</v>
@@ -909,10 +909,10 @@
         <v>9288149</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="5">
         <v>5000000</v>
@@ -923,10 +923,10 @@
         <v>9288150</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="5">
         <v>10671300</v>
@@ -937,10 +937,10 @@
         <v>9288152</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" s="5">
         <v>15130000</v>
@@ -951,10 +951,10 @@
         <v>9288153</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="5">
         <v>3000000</v>
@@ -965,10 +965,10 @@
         <v>9288154</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="5">
         <v>650000</v>
@@ -979,10 +979,10 @@
         <v>9288155</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" s="5">
         <v>5550438.4000000004</v>
@@ -993,10 +993,10 @@
         <v>9288167</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" s="5">
         <v>3773400</v>
@@ -1007,10 +1007,10 @@
         <v>9288168</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" s="5">
         <v>130000000</v>
@@ -1021,10 +1021,10 @@
         <v>9288169</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" s="5">
         <v>16112602.23</v>
@@ -1035,10 +1035,10 @@
         <v>9288176</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" s="5">
         <v>40729352.109999999</v>
@@ -1049,10 +1049,10 @@
         <v>9288177</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" s="5">
         <v>0</v>
@@ -1063,10 +1063,10 @@
         <v>9288178</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30" s="5">
         <v>253000000</v>
@@ -1077,10 +1077,10 @@
         <v>9288179</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" s="5">
         <v>45000000</v>
@@ -1091,10 +1091,10 @@
         <v>9288180</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D32" s="5">
         <v>3072030000</v>
@@ -1105,10 +1105,10 @@
         <v>9288181</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33" s="5">
         <v>75352000</v>
@@ -1120,10 +1120,10 @@
         <v>9288182</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34" s="5">
         <v>7000000</v>
@@ -1134,10 +1134,10 @@
         <v>9288183</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" s="5">
         <v>9302249.2699999996</v>
@@ -1148,10 +1148,10 @@
         <v>9288185</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" s="5">
         <v>2000000</v>
@@ -1162,10 +1162,10 @@
         <v>9288186</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37" s="5">
         <v>3000000</v>
@@ -1176,10 +1176,10 @@
         <v>9288187</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D38" s="5">
         <v>36000000</v>
@@ -1190,10 +1190,10 @@
         <v>9288188</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39" s="5">
         <v>8647600</v>
@@ -1204,10 +1204,10 @@
         <v>9288189</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" s="5">
         <v>300000</v>
@@ -1218,10 +1218,10 @@
         <v>9288190</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D41" s="5">
         <v>100000000</v>
@@ -1232,10 +1232,10 @@
         <v>9288191</v>
       </c>
       <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
         <v>44</v>
-      </c>
-      <c r="C42" t="s">
-        <v>45</v>
       </c>
       <c r="D42" s="5">
         <v>210000000</v>
@@ -1246,10 +1246,10 @@
         <v>9288192</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D43" s="5">
         <v>100000000</v>
@@ -1260,10 +1260,10 @@
         <v>9288193</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D44" s="5">
         <v>3900000</v>
@@ -1274,10 +1274,10 @@
         <v>9288194</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45" s="5">
         <v>3600000</v>
@@ -1288,10 +1288,10 @@
         <v>9288195</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D46" s="5">
         <v>749679</v>
@@ -1302,10 +1302,10 @@
         <v>9288196</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D47" s="5">
         <v>42412000</v>
@@ -1316,10 +1316,10 @@
         <v>9288198</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D48" s="5">
         <v>986059044</v>
@@ -1330,10 +1330,10 @@
         <v>9288210</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D49" s="5">
         <v>2500000</v>
@@ -1344,10 +1344,10 @@
         <v>9288211</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D50" s="5">
         <v>3200000</v>
@@ -1358,10 +1358,10 @@
         <v>9288212</v>
       </c>
       <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
         <v>54</v>
-      </c>
-      <c r="C51" t="s">
-        <v>55</v>
       </c>
       <c r="D51" s="5">
         <v>2427295557.9000001</v>
@@ -1372,10 +1372,10 @@
         <v>9288213</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52" s="5">
         <v>23000005</v>
@@ -1386,10 +1386,10 @@
         <v>9321270</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D53" s="5">
         <v>842212.06</v>
@@ -1400,10 +1400,10 @@
         <v>9334530</v>
       </c>
       <c r="B54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D54" s="6">
         <v>14000000</v>
@@ -1414,10 +1414,10 @@
         <v>9337957</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D55" s="5">
         <v>470156273.05000001</v>
@@ -1428,10 +1428,10 @@
         <v>9341846</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D56" s="5">
         <v>13900000</v>
@@ -1442,10 +1442,10 @@
         <v>9342884</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57" s="5">
         <v>68000000</v>
@@ -1456,10 +1456,10 @@
         <v>9361779</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D58" s="6">
         <v>164460000</v>
@@ -1470,10 +1470,10 @@
         <v>9345390</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" s="6">
         <v>24164127.77</v>
@@ -1485,10 +1485,10 @@
         <v>9345097</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D60" s="6">
         <v>3091752</v>
@@ -1499,10 +1499,10 @@
         <v>9395028</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D61" s="6">
         <v>262717753.97999999</v>
@@ -1513,10 +1513,10 @@
         <v>9428110</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62" s="8">
         <v>200689167</v>
@@ -1527,10 +1527,10 @@
         <v>9428104</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D63" s="6">
         <v>6000000</v>

</xml_diff>

<commit_message>
Revert "altera nomenclatura da planilha xls"
This reverts commit b27f97feb2086cbdeacb165236dab044f90639d3.
</commit_message>
<xml_diff>
--- a/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
+++ b/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\.CGE\transparencia-mg\acordo-judicial-reparacao-vale-projetos\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A377FA-5AB7-4CE8-A058-B288DDD9B75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D332FA3B-0DA0-420C-B859-E3FE121F8D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="867" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,6 +46,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
   <si>
+    <t>projeto</t>
+  </si>
+  <si>
     <t>anexo</t>
   </si>
   <si>
@@ -254,9 +257,6 @@
   </si>
   <si>
     <t>valor_iniciativa</t>
-  </si>
-  <si>
-    <t>iniciativa</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,16 +654,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>70</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -671,10 +671,10 @@
         <v>9288130</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="5">
         <v>1195796000</v>
@@ -685,10 +685,10 @@
         <v>9288130</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="5">
         <v>450000000</v>
@@ -699,10 +699,10 @@
         <v>9288132</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
       </c>
       <c r="D4" s="5">
         <v>270000000</v>
@@ -713,10 +713,10 @@
         <v>9288133</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="5">
         <v>776000000</v>
@@ -727,10 +727,10 @@
         <v>9288134</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="5">
         <v>118860000</v>
@@ -741,10 +741,10 @@
         <v>9288135</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="5">
         <v>1345000</v>
@@ -755,10 +755,10 @@
         <v>9288136</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="5">
         <v>111480000</v>
@@ -769,10 +769,10 @@
         <v>9288137</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="5">
         <v>98100000</v>
@@ -783,10 +783,10 @@
         <v>9288138</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="5">
         <v>38614000</v>
@@ -797,10 +797,10 @@
         <v>9288139</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="5">
         <v>4400000</v>
@@ -811,10 +811,10 @@
         <v>9288141</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="5">
         <v>500000</v>
@@ -825,10 +825,10 @@
         <v>9288142</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="5">
         <v>36712000</v>
@@ -839,10 +839,10 @@
         <v>9288143</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" s="5">
         <v>728000</v>
@@ -853,10 +853,10 @@
         <v>9288144</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" s="5">
         <v>49000000</v>
@@ -867,10 +867,10 @@
         <v>9288145</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" s="5">
         <v>45345000</v>
@@ -881,10 +881,10 @@
         <v>9288147</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="5">
         <v>14817323</v>
@@ -895,10 +895,10 @@
         <v>9288148</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="5">
         <v>4000000</v>
@@ -909,10 +909,10 @@
         <v>9288149</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="5">
         <v>5000000</v>
@@ -923,10 +923,10 @@
         <v>9288150</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" s="5">
         <v>10671300</v>
@@ -937,10 +937,10 @@
         <v>9288152</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21" s="5">
         <v>15130000</v>
@@ -951,10 +951,10 @@
         <v>9288153</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" s="5">
         <v>3000000</v>
@@ -965,10 +965,10 @@
         <v>9288154</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23" s="5">
         <v>650000</v>
@@ -979,10 +979,10 @@
         <v>9288155</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24" s="5">
         <v>5550438.4000000004</v>
@@ -993,10 +993,10 @@
         <v>9288167</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" s="5">
         <v>3773400</v>
@@ -1007,10 +1007,10 @@
         <v>9288168</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" s="5">
         <v>130000000</v>
@@ -1021,10 +1021,10 @@
         <v>9288169</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27" s="5">
         <v>16112602.23</v>
@@ -1035,10 +1035,10 @@
         <v>9288176</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" s="5">
         <v>40729352.109999999</v>
@@ -1049,10 +1049,10 @@
         <v>9288177</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29" s="5">
         <v>0</v>
@@ -1063,10 +1063,10 @@
         <v>9288178</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D30" s="5">
         <v>253000000</v>
@@ -1077,10 +1077,10 @@
         <v>9288179</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" s="5">
         <v>45000000</v>
@@ -1091,10 +1091,10 @@
         <v>9288180</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D32" s="5">
         <v>3072030000</v>
@@ -1105,10 +1105,10 @@
         <v>9288181</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D33" s="5">
         <v>75352000</v>
@@ -1120,10 +1120,10 @@
         <v>9288182</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D34" s="5">
         <v>7000000</v>
@@ -1134,10 +1134,10 @@
         <v>9288183</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35" s="5">
         <v>9302249.2699999996</v>
@@ -1148,10 +1148,10 @@
         <v>9288185</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36" s="5">
         <v>2000000</v>
@@ -1162,10 +1162,10 @@
         <v>9288186</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" s="5">
         <v>3000000</v>
@@ -1176,10 +1176,10 @@
         <v>9288187</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38" s="5">
         <v>36000000</v>
@@ -1190,10 +1190,10 @@
         <v>9288188</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" s="5">
         <v>8647600</v>
@@ -1204,10 +1204,10 @@
         <v>9288189</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40" s="5">
         <v>300000</v>
@@ -1218,10 +1218,10 @@
         <v>9288190</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D41" s="5">
         <v>100000000</v>
@@ -1232,10 +1232,10 @@
         <v>9288191</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D42" s="5">
         <v>210000000</v>
@@ -1246,10 +1246,10 @@
         <v>9288192</v>
       </c>
       <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
         <v>45</v>
-      </c>
-      <c r="C43" t="s">
-        <v>44</v>
       </c>
       <c r="D43" s="5">
         <v>100000000</v>
@@ -1260,10 +1260,10 @@
         <v>9288193</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D44" s="5">
         <v>3900000</v>
@@ -1274,10 +1274,10 @@
         <v>9288194</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D45" s="5">
         <v>3600000</v>
@@ -1288,10 +1288,10 @@
         <v>9288195</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46" s="5">
         <v>749679</v>
@@ -1302,10 +1302,10 @@
         <v>9288196</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47" s="5">
         <v>42412000</v>
@@ -1316,10 +1316,10 @@
         <v>9288198</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D48" s="5">
         <v>986059044</v>
@@ -1330,10 +1330,10 @@
         <v>9288210</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D49" s="5">
         <v>2500000</v>
@@ -1344,10 +1344,10 @@
         <v>9288211</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50" s="5">
         <v>3200000</v>
@@ -1358,10 +1358,10 @@
         <v>9288212</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D51" s="5">
         <v>2427295557.9000001</v>
@@ -1372,10 +1372,10 @@
         <v>9288213</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52" s="5">
         <v>23000005</v>
@@ -1386,10 +1386,10 @@
         <v>9321270</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D53" s="5">
         <v>842212.06</v>
@@ -1400,10 +1400,10 @@
         <v>9334530</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D54" s="6">
         <v>14000000</v>
@@ -1414,10 +1414,10 @@
         <v>9337957</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C55" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D55" s="5">
         <v>470156273.05000001</v>
@@ -1428,10 +1428,10 @@
         <v>9341846</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C56" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D56" s="5">
         <v>13900000</v>
@@ -1442,10 +1442,10 @@
         <v>9342884</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C57" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D57" s="5">
         <v>68000000</v>
@@ -1456,10 +1456,10 @@
         <v>9361779</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D58" s="6">
         <v>164460000</v>
@@ -1470,10 +1470,10 @@
         <v>9345390</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D59" s="6">
         <v>24164127.77</v>
@@ -1485,10 +1485,10 @@
         <v>9345097</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D60" s="6">
         <v>3091752</v>
@@ -1499,10 +1499,10 @@
         <v>9395028</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D61" s="6">
         <v>262717753.97999999</v>
@@ -1513,10 +1513,10 @@
         <v>9428110</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D62" s="8">
         <v>200689167</v>
@@ -1527,10 +1527,10 @@
         <v>9428104</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D63" s="6">
         <v>6000000</v>

</xml_diff>

<commit_message>
Corrige nome na tabela
</commit_message>
<xml_diff>
--- a/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
+++ b/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\.CGE\transparencia-mg\acordo-judicial-reparacao-vale-projetos\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D332FA3B-0DA0-420C-B859-E3FE121F8D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401D091A-12E1-43EF-B1AE-F42F0FD33646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="867" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,9 +46,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
   <si>
-    <t>projeto</t>
-  </si>
-  <si>
     <t>anexo</t>
   </si>
   <si>
@@ -257,6 +254,9 @@
   </si>
   <si>
     <t>valor_iniciativa</t>
+  </si>
+  <si>
+    <t>iniciativa</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,16 +654,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -671,10 +671,10 @@
         <v>9288130</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="5">
         <v>1195796000</v>
@@ -685,10 +685,10 @@
         <v>9288130</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
       <c r="D3" s="5">
         <v>450000000</v>
@@ -699,10 +699,10 @@
         <v>9288132</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5">
         <v>270000000</v>
@@ -713,10 +713,10 @@
         <v>9288133</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5">
         <v>776000000</v>
@@ -727,10 +727,10 @@
         <v>9288134</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5">
         <v>118860000</v>
@@ -741,10 +741,10 @@
         <v>9288135</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="5">
         <v>1345000</v>
@@ -755,10 +755,10 @@
         <v>9288136</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5">
         <v>111480000</v>
@@ -769,10 +769,10 @@
         <v>9288137</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="5">
         <v>98100000</v>
@@ -783,10 +783,10 @@
         <v>9288138</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="5">
         <v>38614000</v>
@@ -797,10 +797,10 @@
         <v>9288139</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="5">
         <v>4400000</v>
@@ -811,10 +811,10 @@
         <v>9288141</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="5">
         <v>500000</v>
@@ -825,10 +825,10 @@
         <v>9288142</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="5">
         <v>36712000</v>
@@ -839,10 +839,10 @@
         <v>9288143</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="5">
         <v>728000</v>
@@ -853,10 +853,10 @@
         <v>9288144</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="5">
         <v>49000000</v>
@@ -867,10 +867,10 @@
         <v>9288145</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="5">
         <v>45345000</v>
@@ -881,10 +881,10 @@
         <v>9288147</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" s="5">
         <v>14817323</v>
@@ -895,10 +895,10 @@
         <v>9288148</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="5">
         <v>4000000</v>
@@ -909,10 +909,10 @@
         <v>9288149</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="5">
         <v>5000000</v>
@@ -923,10 +923,10 @@
         <v>9288150</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="5">
         <v>10671300</v>
@@ -937,10 +937,10 @@
         <v>9288152</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" s="5">
         <v>15130000</v>
@@ -951,10 +951,10 @@
         <v>9288153</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="5">
         <v>3000000</v>
@@ -965,10 +965,10 @@
         <v>9288154</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="5">
         <v>650000</v>
@@ -979,10 +979,10 @@
         <v>9288155</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" s="5">
         <v>5550438.4000000004</v>
@@ -993,10 +993,10 @@
         <v>9288167</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" s="5">
         <v>3773400</v>
@@ -1007,10 +1007,10 @@
         <v>9288168</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" s="5">
         <v>130000000</v>
@@ -1021,10 +1021,10 @@
         <v>9288169</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" s="5">
         <v>16112602.23</v>
@@ -1035,10 +1035,10 @@
         <v>9288176</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" s="5">
         <v>40729352.109999999</v>
@@ -1049,10 +1049,10 @@
         <v>9288177</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" s="5">
         <v>0</v>
@@ -1063,10 +1063,10 @@
         <v>9288178</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30" s="5">
         <v>253000000</v>
@@ -1077,10 +1077,10 @@
         <v>9288179</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" s="5">
         <v>45000000</v>
@@ -1091,10 +1091,10 @@
         <v>9288180</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D32" s="5">
         <v>3072030000</v>
@@ -1105,10 +1105,10 @@
         <v>9288181</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33" s="5">
         <v>75352000</v>
@@ -1120,10 +1120,10 @@
         <v>9288182</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34" s="5">
         <v>7000000</v>
@@ -1134,10 +1134,10 @@
         <v>9288183</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" s="5">
         <v>9302249.2699999996</v>
@@ -1148,10 +1148,10 @@
         <v>9288185</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" s="5">
         <v>2000000</v>
@@ -1162,10 +1162,10 @@
         <v>9288186</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37" s="5">
         <v>3000000</v>
@@ -1176,10 +1176,10 @@
         <v>9288187</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D38" s="5">
         <v>36000000</v>
@@ -1190,10 +1190,10 @@
         <v>9288188</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39" s="5">
         <v>8647600</v>
@@ -1204,10 +1204,10 @@
         <v>9288189</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" s="5">
         <v>300000</v>
@@ -1218,10 +1218,10 @@
         <v>9288190</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D41" s="5">
         <v>100000000</v>
@@ -1232,10 +1232,10 @@
         <v>9288191</v>
       </c>
       <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
         <v>44</v>
-      </c>
-      <c r="C42" t="s">
-        <v>45</v>
       </c>
       <c r="D42" s="5">
         <v>210000000</v>
@@ -1246,10 +1246,10 @@
         <v>9288192</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D43" s="5">
         <v>100000000</v>
@@ -1260,10 +1260,10 @@
         <v>9288193</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D44" s="5">
         <v>3900000</v>
@@ -1274,10 +1274,10 @@
         <v>9288194</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45" s="5">
         <v>3600000</v>
@@ -1288,10 +1288,10 @@
         <v>9288195</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D46" s="5">
         <v>749679</v>
@@ -1302,10 +1302,10 @@
         <v>9288196</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D47" s="5">
         <v>42412000</v>
@@ -1316,10 +1316,10 @@
         <v>9288198</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D48" s="5">
         <v>986059044</v>
@@ -1330,10 +1330,10 @@
         <v>9288210</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D49" s="5">
         <v>2500000</v>
@@ -1344,10 +1344,10 @@
         <v>9288211</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D50" s="5">
         <v>3200000</v>
@@ -1358,10 +1358,10 @@
         <v>9288212</v>
       </c>
       <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
         <v>54</v>
-      </c>
-      <c r="C51" t="s">
-        <v>55</v>
       </c>
       <c r="D51" s="5">
         <v>2427295557.9000001</v>
@@ -1372,10 +1372,10 @@
         <v>9288213</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52" s="5">
         <v>23000005</v>
@@ -1386,10 +1386,10 @@
         <v>9321270</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D53" s="5">
         <v>842212.06</v>
@@ -1400,10 +1400,10 @@
         <v>9334530</v>
       </c>
       <c r="B54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D54" s="6">
         <v>14000000</v>
@@ -1414,10 +1414,10 @@
         <v>9337957</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D55" s="5">
         <v>470156273.05000001</v>
@@ -1428,10 +1428,10 @@
         <v>9341846</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D56" s="5">
         <v>13900000</v>
@@ -1442,10 +1442,10 @@
         <v>9342884</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57" s="5">
         <v>68000000</v>
@@ -1456,10 +1456,10 @@
         <v>9361779</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D58" s="6">
         <v>164460000</v>
@@ -1470,10 +1470,10 @@
         <v>9345390</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" s="6">
         <v>24164127.77</v>
@@ -1485,10 +1485,10 @@
         <v>9345097</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D60" s="6">
         <v>3091752</v>
@@ -1499,10 +1499,10 @@
         <v>9395028</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D61" s="6">
         <v>262717753.97999999</v>
@@ -1513,10 +1513,10 @@
         <v>9428110</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62" s="8">
         <v>200689167</v>
@@ -1527,10 +1527,10 @@
         <v>9428104</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D63" s="6">
         <v>6000000</v>

</xml_diff>

<commit_message>
Inclui projeto transporte metropolitano - '0000000'
Incluí projeto transporte metropolitano com número provisório do instrumento '0000000'
</commit_message>
<xml_diff>
--- a/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
+++ b/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27929"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\.CGE\transparencia-mg\acordo-judicial-reparacao-vale-projetos\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401D091A-12E1-43EF-B1AE-F42F0FD33646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF8207D2-F431-4443-8C8E-823816D2366B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="867" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,11 +44,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
+  <si>
+    <t>codigo_iniciativa</t>
+  </si>
+  <si>
+    <t>iniciativa</t>
+  </si>
   <si>
     <t>anexo</t>
   </si>
   <si>
+    <t>valor_iniciativa</t>
+  </si>
+  <si>
     <t>Melhoria da infraestrutura dos municípios</t>
   </si>
   <si>
@@ -250,13 +259,13 @@
     <t>Melhoria da infraestrutura dos municípios – Adequação de serviços de transporte fluvial em Morada Nova de Minas</t>
   </si>
   <si>
-    <t>codigo_iniciativa</t>
-  </si>
-  <si>
-    <t>valor_iniciativa</t>
-  </si>
-  <si>
-    <t>iniciativa</t>
+    <t>0000000</t>
+  </si>
+  <si>
+    <t>Melhoria da infraestrutura dos municípios – Fortalecimento do transporte metropolitano</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -267,7 +276,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,6 +342,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -632,910 +644,925 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="62.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="62.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="45" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="3"/>
-    <col min="6" max="6" width="16.5546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="3"/>
-    <col min="8" max="8" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.88671875" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="3"/>
+    <col min="4" max="4" width="20.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="16.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4">
         <v>9288130</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2" s="5">
         <v>1195796000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="4">
         <v>9288130</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D3" s="5">
         <v>450000000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="4">
         <v>9288132</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5">
-        <v>270000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>410000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="4">
         <v>9288133</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D5" s="5">
-        <v>776000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>887000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="4">
         <v>9288134</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6" s="5">
         <v>118860000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="4">
         <v>9288135</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D7" s="5">
         <v>1345000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="4">
         <v>9288136</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D8" s="5">
         <v>111480000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="4">
         <v>9288137</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D9" s="5">
         <v>98100000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="4">
         <v>9288138</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D10" s="5">
         <v>38614000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="4">
         <v>9288139</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D11" s="5">
         <v>4400000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="4">
         <v>9288141</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D12" s="5">
         <v>500000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="4">
         <v>9288142</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D13" s="5">
         <v>36712000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="4">
         <v>9288143</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14" s="5">
         <v>728000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="4">
         <v>9288144</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" s="5">
         <v>49000000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="4">
         <v>9288145</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16" s="5">
         <v>45345000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="4">
         <v>9288147</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17" s="5">
         <v>14817323</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="4">
         <v>9288148</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D18" s="5">
         <v>4000000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="4">
         <v>9288149</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19" s="5">
         <v>5000000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="4">
         <v>9288150</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D20" s="5">
         <v>10671300</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="4">
         <v>9288152</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D21" s="5">
         <v>15130000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="4">
         <v>9288153</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D22" s="5">
         <v>3000000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="4">
         <v>9288154</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D23" s="5">
         <v>650000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="4">
         <v>9288155</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D24" s="5">
         <v>5550438.4000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="4">
         <v>9288167</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D25" s="5">
         <v>3773400</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="4">
         <v>9288168</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D26" s="5">
         <v>130000000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="4">
         <v>9288169</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D27" s="5">
         <v>16112602.23</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="4">
         <v>9288176</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D28" s="5">
         <v>40729352.109999999</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="4">
         <v>9288177</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D29" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="4">
         <v>9288178</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D30" s="5">
         <v>253000000</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="4">
         <v>9288179</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D31" s="5">
         <v>45000000</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="4">
         <v>9288180</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D32" s="5">
         <v>3072030000</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="4">
         <v>9288181</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D33" s="5">
         <v>75352000</v>
       </c>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="4">
         <v>9288182</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D34" s="5">
         <v>7000000</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="4">
         <v>9288183</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D35" s="5">
-        <v>9302249.2699999996</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="4">
         <v>9288185</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D36" s="5">
         <v>2000000</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="4">
         <v>9288186</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D37" s="5">
         <v>3000000</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="4">
         <v>9288187</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D38" s="5">
         <v>36000000</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="4">
         <v>9288188</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D39" s="5">
         <v>8647600</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="4">
         <v>9288189</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D40" s="5">
         <v>300000</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="4">
         <v>9288190</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D41" s="5">
         <v>100000000</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="4">
         <v>9288191</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D42" s="5">
         <v>210000000</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="4">
         <v>9288192</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D43" s="5">
         <v>100000000</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="4">
         <v>9288193</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C44" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D44" s="5">
         <v>3900000</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="4">
         <v>9288194</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D45" s="5">
         <v>3600000</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="4">
         <v>9288195</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D46" s="5">
         <v>749679</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="4">
         <v>9288196</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C47" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D47" s="5">
         <v>42412000</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="4">
         <v>9288198</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C48" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D48" s="5">
         <v>986059044</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="4">
         <v>9288210</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D49" s="5">
-        <v>2500000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2300000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="4">
         <v>9288211</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D50" s="5">
-        <v>3200000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3400000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="4">
         <v>9288212</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D51" s="5">
         <v>2427295557.9000001</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="4">
         <v>9288213</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D52" s="5">
         <v>23000005</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="4">
         <v>9321270</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D53" s="5">
         <v>842212.06</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A54">
         <v>9334530</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D54" s="6">
         <v>14000000</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A55">
         <v>9337957</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C55" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D55" s="5">
         <v>470156273.05000001</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A56">
         <v>9341846</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D56" s="5">
         <v>13900000</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A57">
         <v>9342884</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D57" s="5">
         <v>68000000</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="7">
         <v>9361779</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D58" s="6">
         <v>164460000</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="7">
         <v>9345390</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D59" s="6">
         <v>24164127.77</v>
       </c>
       <c r="F59" s="9"/>
     </row>
-    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="28.9">
       <c r="A60" s="7">
         <v>9345097</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D60" s="6">
         <v>3091752</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="28.9">
       <c r="A61" s="7">
         <v>9395028</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D61" s="6">
         <v>262717753.97999999</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="28.9">
       <c r="A62" s="7">
         <v>9428110</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D62" s="8">
         <v>200689167</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="28.9">
       <c r="A63" s="7">
         <v>9428104</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D63" s="6">
         <v>6000000</v>
       </c>
     </row>
+    <row r="64" spans="1:6" ht="30.75">
+      <c r="A64" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D64" s="6">
+        <v>380000000</v>
+      </c>
+    </row>
+    <row r="65" ht="15"/>
   </sheetData>
   <autoFilter ref="A1:H63" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D58">

</xml_diff>

<commit_message>
Add instrumento - deliberação 21
</commit_message>
<xml_diff>
--- a/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
+++ b/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28209"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\.CGE\transparencia-mg\acordo-judicial-reparacao-vale-projetos\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB17EB8F-F775-401D-A29D-CA172CB46743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DD3A432-DA27-4CA3-BD8E-76713D7823EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="867" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="75">
   <si>
     <t>codigo_iniciativa</t>
   </si>
@@ -127,7 +127,7 @@
     <t>Pesquisas, Tendências e Monitoramento da Cultura e do Turismo</t>
   </si>
   <si>
-    <t>Plano de Desenvolvimento Integrado do Turismo em Minas Gerais</t>
+    <t>Plano Diretor do Turismo Verde em Minas Gerais - Plano de Desenvolvimento Integrado do Turismo Sustentável de Minas Gerais</t>
   </si>
   <si>
     <t>Fortalecimento e reestruturação tecnológica da Controladoria Geral do Estado</t>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>Melhoria da infraestrutura dos municípios – Melhoria da oferta e do acesso à saúde da população de Juiz de Fora e Zona da Mata</t>
   </si>
 </sst>
 </file>
@@ -276,7 +279,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,27 +647,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A56" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="62.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="62.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="45" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="3"/>
-    <col min="6" max="6" width="16.5546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="3"/>
-    <col min="8" max="8" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.88671875" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="3"/>
+    <col min="4" max="4" width="20.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="16.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4">
         <v>9288130</v>
       </c>
@@ -692,7 +695,7 @@
         <v>1195796000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="4">
         <v>9288130</v>
       </c>
@@ -706,7 +709,7 @@
         <v>450000000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="4">
         <v>9288132</v>
       </c>
@@ -720,7 +723,7 @@
         <v>410000000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="4">
         <v>9288133</v>
       </c>
@@ -734,7 +737,7 @@
         <v>887000000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="4">
         <v>9288134</v>
       </c>
@@ -748,7 +751,7 @@
         <v>118860000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="4">
         <v>9288135</v>
       </c>
@@ -762,7 +765,7 @@
         <v>1345000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="4">
         <v>9288136</v>
       </c>
@@ -776,7 +779,7 @@
         <v>111480000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="4">
         <v>9288137</v>
       </c>
@@ -790,7 +793,7 @@
         <v>98100000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="4">
         <v>9288138</v>
       </c>
@@ -804,7 +807,7 @@
         <v>38614000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="4">
         <v>9288139</v>
       </c>
@@ -818,7 +821,7 @@
         <v>4400000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="4">
         <v>9288141</v>
       </c>
@@ -832,7 +835,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="4">
         <v>9288142</v>
       </c>
@@ -846,7 +849,7 @@
         <v>36712000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="4">
         <v>9288143</v>
       </c>
@@ -860,7 +863,7 @@
         <v>728000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="4">
         <v>9288144</v>
       </c>
@@ -874,7 +877,7 @@
         <v>49000000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="4">
         <v>9288145</v>
       </c>
@@ -888,7 +891,7 @@
         <v>45345000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="4">
         <v>9288147</v>
       </c>
@@ -902,7 +905,7 @@
         <v>14817323</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="4">
         <v>9288148</v>
       </c>
@@ -916,7 +919,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="4">
         <v>9288149</v>
       </c>
@@ -930,7 +933,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="4">
         <v>9288150</v>
       </c>
@@ -944,7 +947,7 @@
         <v>10671300</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="4">
         <v>9288152</v>
       </c>
@@ -958,7 +961,7 @@
         <v>15130000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="4">
         <v>9288153</v>
       </c>
@@ -972,7 +975,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="4">
         <v>9288154</v>
       </c>
@@ -986,7 +989,7 @@
         <v>650000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="4">
         <v>9288155</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>5550438.4000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="4">
         <v>9288167</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>3773400</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="4">
         <v>9288168</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>130000000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="4">
         <v>9288169</v>
       </c>
@@ -1042,7 +1045,7 @@
         <v>16112602.23</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="4">
         <v>9288176</v>
       </c>
@@ -1056,7 +1059,7 @@
         <v>40729352.109999999</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="4">
         <v>9288177</v>
       </c>
@@ -1070,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="4">
         <v>9288178</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>253000000</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="4">
         <v>9288179</v>
       </c>
@@ -1098,7 +1101,7 @@
         <v>45000000</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="4">
         <v>9288180</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>3072030000</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="4">
         <v>9288181</v>
       </c>
@@ -1127,7 +1130,7 @@
       </c>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="4">
         <v>9288182</v>
       </c>
@@ -1141,7 +1144,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="4">
         <v>9288183</v>
       </c>
@@ -1155,7 +1158,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="4">
         <v>9288185</v>
       </c>
@@ -1169,7 +1172,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="4">
         <v>9288186</v>
       </c>
@@ -1183,7 +1186,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="4">
         <v>9288187</v>
       </c>
@@ -1197,7 +1200,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="4">
         <v>9288188</v>
       </c>
@@ -1211,7 +1214,7 @@
         <v>8647600</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="4">
         <v>9288189</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="4">
         <v>9288190</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="4">
         <v>9288191</v>
       </c>
@@ -1253,7 +1256,7 @@
         <v>210000000</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="4">
         <v>9288192</v>
       </c>
@@ -1267,7 +1270,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="4">
         <v>9288193</v>
       </c>
@@ -1281,7 +1284,7 @@
         <v>3900000</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="4">
         <v>9288194</v>
       </c>
@@ -1295,7 +1298,7 @@
         <v>3600000</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="4">
         <v>9288195</v>
       </c>
@@ -1309,7 +1312,7 @@
         <v>749679</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="4">
         <v>9288196</v>
       </c>
@@ -1323,7 +1326,7 @@
         <v>42412000</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="4">
         <v>9288198</v>
       </c>
@@ -1334,10 +1337,10 @@
         <v>5</v>
       </c>
       <c r="D48" s="5">
-        <v>986059044</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>836059044</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="4">
         <v>9288210</v>
       </c>
@@ -1351,7 +1354,7 @@
         <v>2300000</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="4">
         <v>9288211</v>
       </c>
@@ -1365,7 +1368,7 @@
         <v>3400000</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="4">
         <v>9288212</v>
       </c>
@@ -1379,7 +1382,7 @@
         <v>2427295557.9000001</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="4">
         <v>9288213</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>23000005</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="4">
         <v>9321270</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>842212.06</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A54">
         <v>9334530</v>
       </c>
@@ -1421,7 +1424,7 @@
         <v>14000000</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A55">
         <v>9337957</v>
       </c>
@@ -1435,7 +1438,7 @@
         <v>470156273.05000001</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A56">
         <v>9341846</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>13900000</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A57">
         <v>9342884</v>
       </c>
@@ -1463,7 +1466,7 @@
         <v>68000000</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="7">
         <v>9361779</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>164460000</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="7">
         <v>9345390</v>
       </c>
@@ -1492,7 +1495,7 @@
       </c>
       <c r="F59" s="9"/>
     </row>
-    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="30.75">
       <c r="A60" s="7">
         <v>9345097</v>
       </c>
@@ -1506,7 +1509,7 @@
         <v>3091752</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="30.75">
       <c r="A61" s="7">
         <v>9395028</v>
       </c>
@@ -1520,7 +1523,7 @@
         <v>262717753.97999999</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="30.75">
       <c r="A62" s="7">
         <v>9428110</v>
       </c>
@@ -1534,7 +1537,7 @@
         <v>200689167</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="30.75">
       <c r="A63" s="7">
         <v>9428104</v>
       </c>
@@ -1548,7 +1551,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="30.75">
       <c r="A64" s="11" t="s">
         <v>71</v>
       </c>
@@ -1562,6 +1565,21 @@
         <v>380000000</v>
       </c>
     </row>
+    <row r="65" spans="1:4" ht="30.75">
+      <c r="A65" s="7">
+        <v>9440688</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="6">
+        <v>150000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15"/>
   </sheetData>
   <autoFilter ref="A1:H63" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D58">

</xml_diff>

<commit_message>
Corrige valor projeto intervenções bacia (0,01)
Erro de arredondamento corrigido
</commit_message>
<xml_diff>
--- a/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
+++ b/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\.CGE\transparencia-mg\acordo-judicial-reparacao-vale-projetos\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DD3A432-DA27-4CA3-BD8E-76713D7823EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB90BBF6-D26F-4ED9-ADAB-1777F3F2802C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="867" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A56" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -1379,7 +1379,7 @@
         <v>57</v>
       </c>
       <c r="D51" s="5">
-        <v>2427295557.9000001</v>
+        <v>2427295557.8899999</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="20.100000000000001" customHeight="1">

</xml_diff>

<commit_message>
Atualiza conforme deliberação 22
</commit_message>
<xml_diff>
--- a/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
+++ b/upload/iniciativas_acordo_judicial_reparacao_vale.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28417"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\.CGE\transparencia-mg\acordo-judicial-reparacao-vale-projetos\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB90BBF6-D26F-4ED9-ADAB-1777F3F2802C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92D53E08-1072-4A35-9C77-5B2FA58FC376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="867" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1562,7 +1562,7 @@
         <v>73</v>
       </c>
       <c r="D64" s="6">
-        <v>380000000</v>
+        <v>393211725.25</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="30.75">

</xml_diff>